<commit_message>
Updated examples and unit tests.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Columns/DeletingColumns.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Columns/DeletingColumns.xlsx
@@ -380,7 +380,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B2"/>
+  <x:dimension ref="A1:H3"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
@@ -389,8 +389,8 @@
     <x:col min="1" max="16384" width="9.850625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:2"/>
-    <x:row r="2" spans="1:2">
+    <x:row r="1" spans="1:8"/>
+    <x:row r="2" spans="1:8">
       <x:c r="A2" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -398,7 +398,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:2"/>
+    <x:row r="3" spans="1:8"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>